<commit_message>
Gauss points now fully-defined and able to be plotted by mesh.plot()'
</commit_message>
<xml_diff>
--- a/examples/Nodle import/NODLE_demo.xlsx
+++ b/examples/Nodle import/NODLE_demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rihy\DynSys\examples\Nodle import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{DD47F4FA-3641-421E-A50F-5C8B9FB3319C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB67571-8366-4200-8940-10296592ABA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="405" windowWidth="10860" windowHeight="6150" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="405" windowWidth="10860" windowHeight="6150" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="56" r:id="rId1"/>
@@ -1185,6 +1185,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1215,13 +1222,6 @@
     <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2407,10 +2407,10 @@
       <c r="B4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="16" t="s">
         <v>83</v>
       </c>
@@ -2517,10 +2517,10 @@
       <c r="C4" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="61"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="16" t="s">
         <v>103</v>
       </c>
@@ -2637,10 +2637,10 @@
       <c r="D4" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="61"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="16" t="s">
         <v>110</v>
       </c>
@@ -2765,10 +2765,10 @@
       <c r="F4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="61"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -3074,16 +3074,16 @@
       <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="60" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="J4" s="62"/>
-      <c r="K4" s="61"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3213,16 +3213,16 @@
       <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="60" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="J4" s="62"/>
-      <c r="K4" s="61"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="64"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3358,16 +3358,16 @@
       <c r="F4" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="60" t="s">
+      <c r="H4" s="65"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="61"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="64"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3709,16 +3709,16 @@
       <c r="F4" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="60" t="s">
+      <c r="H4" s="65"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="K4" s="62"/>
-      <c r="L4" s="62"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
       <c r="M4" s="15" t="s">
         <v>162</v>
       </c>
@@ -3861,11 +3861,11 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="15" t="s">
         <v>231</v>
       </c>
@@ -4105,26 +4105,26 @@
       <c r="C4" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="60" t="s">
+      <c r="E4" s="64"/>
+      <c r="F4" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="61"/>
-      <c r="H4" s="60" t="s">
+      <c r="G4" s="64"/>
+      <c r="H4" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="60" t="s">
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="60" t="s">
+      <c r="K4" s="64"/>
+      <c r="L4" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="M4" s="61"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -4295,20 +4295,20 @@
       <c r="H4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="60" t="s">
+      <c r="I4" s="63" t="s">
         <v>190</v>
       </c>
-      <c r="J4" s="61"/>
-      <c r="K4" s="60" t="s">
+      <c r="J4" s="64"/>
+      <c r="K4" s="63" t="s">
         <v>193</v>
       </c>
-      <c r="L4" s="62"/>
-      <c r="M4" s="62"/>
-      <c r="N4" s="62"/>
-      <c r="O4" s="62"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="61"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="64"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -4421,8 +4421,8 @@
       <c r="C5" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -4430,8 +4430,8 @@
       <c r="C6" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -4439,8 +4439,8 @@
       <c r="C7" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="54"/>
@@ -4830,16 +4830,16 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="67" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="70" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="72"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -4954,20 +4954,20 @@
       <c r="C4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="67" t="s">
+      <c r="E4" s="71"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="67" t="s">
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="70" t="s">
         <v>214</v>
       </c>
-      <c r="K4" s="69"/>
+      <c r="K4" s="72"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5145,16 +5145,16 @@
       <c r="C4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="67" t="s">
+      <c r="E4" s="71"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5260,16 +5260,16 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="68"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="67" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="70" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="72"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5537,10 +5537,10 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="61"/>
+      <c r="C4" s="64"/>
       <c r="D4" s="45" t="s">
         <v>22</v>
       </c>
@@ -5671,25 +5671,25 @@
       <c r="D4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="61"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="60" t="s">
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="61"/>
-      <c r="L4" s="60" t="s">
+      <c r="K4" s="64"/>
+      <c r="L4" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="61"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5756,9 +5756,9 @@
   </sheetPr>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5805,11 +5805,11 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="61"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="15" t="s">
         <v>83</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>302</v>
       </c>
       <c r="C14" s="59">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="D14" s="59">
         <v>-2</v>
@@ -5968,7 +5968,7 @@
         <v>301</v>
       </c>
       <c r="C15" s="59">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="D15" s="59">
         <v>-2</v>
@@ -6001,7 +6001,7 @@
   </sheetPr>
   <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -6066,25 +6066,25 @@
       <c r="B4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="60" t="s">
+      <c r="D4" s="64"/>
+      <c r="E4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="61"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="60" t="s">
+      <c r="H4" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="61"/>
-      <c r="J4" s="60" t="s">
+      <c r="I4" s="64"/>
+      <c r="J4" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="61"/>
+      <c r="K4" s="64"/>
       <c r="L4" s="15" t="s">
         <v>89</v>
       </c>
@@ -6125,7 +6125,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="71" t="s">
+      <c r="B6" s="61" t="s">
         <v>240</v>
       </c>
     </row>
@@ -6192,7 +6192,7 @@
       <c r="K10" s="59"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="61" t="s">
         <v>241</v>
       </c>
       <c r="C11" s="59"/>
@@ -6234,7 +6234,7 @@
       <c r="K13" s="59"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="70">
+      <c r="B14" s="60">
         <v>7</v>
       </c>
       <c r="C14" s="21">
@@ -6248,7 +6248,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="62" t="s">
         <v>242</v>
       </c>
       <c r="C15" s="59"/>
@@ -6383,11 +6383,11 @@
       <c r="F4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="60" t="s">
+      <c r="G4" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="62"/>
-      <c r="I4" s="61"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="64"/>
       <c r="J4" s="15" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
NODLE results file added to example
</commit_message>
<xml_diff>
--- a/examples/Nodle import/NODLE_demo.xlsx
+++ b/examples/Nodle import/NODLE_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rihy\DynSys\examples\Nodle import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB67571-8366-4200-8940-10296592ABA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AD90EB-3978-497A-AE19-F3B7AA2B66F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="405" windowWidth="10860" windowHeight="6150" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="405" windowWidth="10860" windowHeight="6150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="56" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="249">
   <si>
     <t>Job number:</t>
   </si>
@@ -822,6 +822,24 @@
   </si>
   <si>
     <t>:Members with skew angles</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Demo model</t>
+  </si>
+  <si>
+    <t>Concrete</t>
+  </si>
+  <si>
+    <t>Nodle DL</t>
+  </si>
+  <si>
+    <t>Nominal DL</t>
+  </si>
+  <si>
+    <t>SDL</t>
   </si>
 </sst>
 </file>
@@ -1058,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1192,6 +1210,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1220,6 +1241,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1679,7 +1712,9 @@
   </sheetPr>
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2361,7 +2396,7 @@
     <tabColor indexed="27"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G5"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2407,10 +2442,10 @@
       <c r="B4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="D4" s="64"/>
+      <c r="D4" s="65"/>
       <c r="E4" s="16" t="s">
         <v>83</v>
       </c>
@@ -2436,6 +2471,9 @@
         <v>93</v>
       </c>
       <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2517,10 +2555,10 @@
       <c r="C4" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="16" t="s">
         <v>103</v>
       </c>
@@ -2637,10 +2675,10 @@
       <c r="D4" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="16" t="s">
         <v>110</v>
       </c>
@@ -2765,10 +2803,10 @@
       <c r="F4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="H4" s="64"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="25"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
@@ -2933,7 +2971,7 @@
     <tabColor indexed="35"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C5"/>
+  <dimension ref="B1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2980,6 +3018,22 @@
       </c>
       <c r="C5" s="17" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="21">
+        <v>2</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -3074,16 +3128,16 @@
       <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="64" t="s">
         <v>149</v>
       </c>
-      <c r="G4" s="65"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="63" t="s">
+      <c r="G4" s="66"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="64" t="s">
         <v>150</v>
       </c>
-      <c r="J4" s="65"/>
-      <c r="K4" s="64"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3140,7 +3194,7 @@
     <tabColor indexed="35"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K5"/>
+  <dimension ref="B1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
@@ -3213,16 +3267,16 @@
       <c r="E4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="65"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="63" t="s">
+      <c r="G4" s="66"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="J4" s="65"/>
-      <c r="K4" s="64"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3254,6 +3308,17 @@
       </c>
       <c r="K5" s="17" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>2</v>
+      </c>
+      <c r="C6" s="21">
+        <v>202</v>
+      </c>
+      <c r="H6" s="21">
+        <v>-10</v>
       </c>
     </row>
   </sheetData>
@@ -3358,16 +3423,16 @@
       <c r="F4" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="63" t="s">
+      <c r="H4" s="66"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="64" t="s">
         <v>153</v>
       </c>
-      <c r="K4" s="65"/>
-      <c r="L4" s="64"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -3506,7 +3571,9 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3599,7 +3666,9 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D12" s="10"/>
+      <c r="D12" s="76" t="s">
+        <v>244</v>
+      </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3709,16 +3778,16 @@
       <c r="F4" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="63" t="s">
+      <c r="H4" s="66"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
       <c r="M4" s="15" t="s">
         <v>162</v>
       </c>
@@ -3861,11 +3930,11 @@
       <c r="E4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="64" t="s">
         <v>230</v>
       </c>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="15" t="s">
         <v>231</v>
       </c>
@@ -4031,7 +4100,7 @@
     <tabColor indexed="35"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M5"/>
+  <dimension ref="B1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
@@ -4105,26 +4174,26 @@
       <c r="C4" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="64" t="s">
         <v>183</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="63" t="s">
+      <c r="E4" s="65"/>
+      <c r="F4" s="64" t="s">
         <v>182</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="63" t="s">
+      <c r="G4" s="65"/>
+      <c r="H4" s="64" t="s">
         <v>181</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="63" t="s">
+      <c r="I4" s="65"/>
+      <c r="J4" s="64" t="s">
         <v>180</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="63" t="s">
+      <c r="K4" s="65"/>
+      <c r="L4" s="64" t="s">
         <v>179</v>
       </c>
-      <c r="M4" s="64"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -4162,6 +4231,26 @@
       </c>
       <c r="M5" s="26" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>247</v>
+      </c>
+      <c r="D6" s="21">
+        <v>1</v>
+      </c>
+      <c r="E6" s="21">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21">
+        <v>2</v>
+      </c>
+      <c r="G6" s="21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4295,20 +4384,20 @@
       <c r="H4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="63" t="s">
+      <c r="I4" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="J4" s="64"/>
-      <c r="K4" s="63" t="s">
+      <c r="J4" s="65"/>
+      <c r="K4" s="64" t="s">
         <v>193</v>
       </c>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="64"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="65"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
@@ -4421,8 +4510,8 @@
       <c r="C5" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="29"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
@@ -4430,8 +4519,8 @@
       <c r="C6" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="68"/>
       <c r="F6" s="29"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
@@ -4439,8 +4528,8 @@
       <c r="C7" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="68"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="54"/>
@@ -4830,16 +4919,16 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="71" t="s">
         <v>205</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="70" t="s">
+      <c r="D4" s="72"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="71" t="s">
         <v>150</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -4954,20 +5043,20 @@
       <c r="C4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="70" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="70" t="s">
+      <c r="H4" s="72"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="71" t="s">
         <v>214</v>
       </c>
-      <c r="K4" s="72"/>
+      <c r="K4" s="73"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5145,16 +5234,16 @@
       <c r="C4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="70" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5260,16 +5349,16 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="71" t="s">
         <v>152</v>
       </c>
-      <c r="D4" s="71"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="70" t="s">
+      <c r="D4" s="72"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="71" t="s">
         <v>153</v>
       </c>
-      <c r="G4" s="71"/>
-      <c r="H4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5319,7 +5408,9 @@
   </sheetPr>
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5369,13 +5460,17 @@
       <c r="C8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="11"/>
+      <c r="D8" s="75" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="75" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
@@ -5469,7 +5564,9 @@
       <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -5490,7 +5587,7 @@
     <tabColor indexed="27"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:H5"/>
+  <dimension ref="B1:H7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -5537,10 +5634,10 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="64"/>
+      <c r="C4" s="65"/>
       <c r="D4" s="45" t="s">
         <v>22</v>
       </c>
@@ -5572,6 +5669,40 @@
       </c>
       <c r="G5" s="17" t="s">
         <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="60" t="s">
+        <v>243</v>
+      </c>
+      <c r="D6" s="74">
+        <v>205000000</v>
+      </c>
+      <c r="E6" s="74">
+        <v>81000000</v>
+      </c>
+      <c r="F6" s="21">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="21">
+        <v>2</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="74">
+        <v>35000000</v>
+      </c>
+      <c r="E7" s="74">
+        <v>18000000</v>
+      </c>
+      <c r="F7" s="21">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -5596,7 +5727,7 @@
     <tabColor indexed="27"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:N5"/>
+  <dimension ref="B1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
@@ -5671,25 +5802,25 @@
       <c r="D4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="63" t="s">
+      <c r="H4" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="63" t="s">
+      <c r="I4" s="65"/>
+      <c r="J4" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="64"/>
-      <c r="L4" s="63" t="s">
+      <c r="K4" s="65"/>
+      <c r="L4" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="64"/>
+      <c r="M4" s="65"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
@@ -5727,6 +5858,84 @@
       </c>
       <c r="M5" s="18" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="21">
+        <v>1</v>
+      </c>
+      <c r="D6" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F6" s="63">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G6" s="74">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H6" s="74">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I6" s="74">
+        <v>3.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="21">
+        <v>2</v>
+      </c>
+      <c r="C7" s="21">
+        <v>2</v>
+      </c>
+      <c r="D7" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="21">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0.06</v>
+      </c>
+      <c r="G7" s="74">
+        <v>1E-4</v>
+      </c>
+      <c r="H7" s="74">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="I7" s="74">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="21">
+        <v>3</v>
+      </c>
+      <c r="C8" s="21">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21">
+        <v>0.02</v>
+      </c>
+      <c r="E8" s="63">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F8" s="63">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G8" s="74">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="H8" s="74">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="I8" s="74">
+        <v>6.0000000000000002E-5</v>
       </c>
     </row>
   </sheetData>
@@ -5756,9 +5965,9 @@
   </sheetPr>
   <dimension ref="B1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5805,11 +6014,11 @@
       <c r="B4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="65"/>
-      <c r="E4" s="64"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="65"/>
       <c r="F4" s="15" t="s">
         <v>83</v>
       </c>
@@ -6005,7 +6214,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6066,25 +6275,25 @@
       <c r="B4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="63" t="s">
+      <c r="D4" s="65"/>
+      <c r="E4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="65"/>
       <c r="G4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="63" t="s">
+      <c r="H4" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="64"/>
-      <c r="J4" s="63" t="s">
+      <c r="I4" s="65"/>
+      <c r="J4" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="K4" s="64"/>
+      <c r="K4" s="65"/>
       <c r="L4" s="15" t="s">
         <v>89</v>
       </c>
@@ -6266,7 +6475,7 @@
         <v>302</v>
       </c>
       <c r="E16" s="59">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
@@ -6280,7 +6489,7 @@
         <v>301</v>
       </c>
       <c r="E17" s="59">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6308,7 +6517,7 @@
     <tabColor indexed="27"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:K5"/>
+  <dimension ref="B1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
@@ -6383,11 +6592,11 @@
       <c r="F4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="63" t="s">
+      <c r="G4" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="H4" s="65"/>
-      <c r="I4" s="64"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="65"/>
       <c r="J4" s="15" t="s">
         <v>89</v>
       </c>
@@ -6419,6 +6628,22 @@
       </c>
       <c r="J5" s="17" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="21">
+        <v>101</v>
+      </c>
+      <c r="C6" s="21">
+        <v>111111</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B7" s="21">
+        <v>301</v>
+      </c>
+      <c r="C7" s="21">
+        <v>111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>